<commit_message>
In the se-space-check tool, use the option space of lcg-insoties rather than option se. Option space reports new attributes GlueSA*OnlineSize instad of deprecated attributes GlueSAState*Space.
</commit_message>
<xml_diff>
--- a/SE/se-space-check-1.0/results/results.xlsx
+++ b/SE/se-space-check-1.0/results/results.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="133">
   <si>
     <t>arc.univ.kiev.ua</t>
   </si>
@@ -474,6 +474,27 @@
   </si>
   <si>
     <t>duplicate entity fixed</t>
+  </si>
+  <si>
+    <t>lcg-infosites se</t>
+  </si>
+  <si>
+    <t>on hold, upgrading  SE from dCache 1.9.5 to 1.9.12</t>
+  </si>
+  <si>
+    <t>1 r/o pool reported with 09 capacity</t>
+  </si>
+  <si>
+    <t>2 pools, prob. normal</t>
+  </si>
+  <si>
+    <t>Inconsistent with Gstat</t>
+  </si>
+  <si>
+    <t>reported twice with space, once with se</t>
+  </si>
+  <si>
+    <t>fixed, old disk pool defined in the SE with non filesystems attached</t>
   </si>
 </sst>
 </file>
@@ -702,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -818,6 +839,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -836,11 +865,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1175,24 +1216,24 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="26.25" customHeight="1">
       <c r="A1"/>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="39" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="26.25" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -6738,10 +6779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6763,24 +6804,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="D1" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="39" t="s">
+      <c r="D1" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
@@ -7007,7 +7048,9 @@
       <c r="A7" s="9">
         <v>75956</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
@@ -7099,79 +7142,81 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="12" customFormat="1">
-      <c r="A9" s="9">
+    <row r="9" spans="1:15" s="32" customFormat="1">
+      <c r="A9" s="30">
         <v>75957</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
+      <c r="G9" s="32">
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
         <v>3567</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="32">
         <v>2867</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="32">
         <v>6435</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="32">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="16" customFormat="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15" t="s">
+    <row r="10" spans="1:15" s="35" customFormat="1">
+      <c r="A10" s="33"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="35">
         <v>3567</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="35">
         <v>2867</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="35">
         <v>6435</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="35">
         <v>44</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="35">
         <v>3567</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="35">
         <v>2867</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="35">
         <v>6435</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="35">
         <v>44</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="35">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -7180,7 +7225,7 @@
       <c r="A11" s="30">
         <v>75959</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="47" t="s">
         <v>123</v>
       </c>
       <c r="C11" s="31" t="s">
@@ -7229,7 +7274,7 @@
     </row>
     <row r="12" spans="1:15" s="35" customFormat="1">
       <c r="A12" s="33"/>
-      <c r="B12" s="44"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="34" t="s">
         <v>38</v>
       </c>
@@ -7278,7 +7323,9 @@
       <c r="A13" s="9">
         <v>75960</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="49" t="s">
+        <v>127</v>
+      </c>
       <c r="C13" s="11" t="s">
         <v>41</v>
       </c>
@@ -7306,7 +7353,7 @@
     </row>
     <row r="14" spans="1:15" s="16" customFormat="1">
       <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="15" t="s">
         <v>41</v>
       </c>
@@ -7512,7 +7559,9 @@
       <c r="A19" s="9">
         <v>75963</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="C19" s="11" t="s">
         <v>64</v>
       </c>
@@ -7608,7 +7657,9 @@
       <c r="A21" s="9">
         <v>75964</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B21" s="49" t="s">
+        <v>128</v>
+      </c>
       <c r="C21" s="11" t="s">
         <v>70</v>
       </c>
@@ -7639,7 +7690,7 @@
     </row>
     <row r="22" spans="1:15" s="16" customFormat="1">
       <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="15" t="s">
         <v>70</v>
       </c>
@@ -7784,7 +7835,9 @@
       <c r="A25" s="9">
         <v>75965</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="C25" s="11" t="s">
         <v>87</v>
       </c>
@@ -7880,7 +7933,9 @@
       <c r="A27" s="9">
         <v>75966</v>
       </c>
-      <c r="B27" s="10"/>
+      <c r="B27" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="C27" s="11" t="s">
         <v>88</v>
       </c>
@@ -7976,7 +8031,9 @@
       <c r="A29" s="19">
         <v>75970</v>
       </c>
-      <c r="B29" s="20"/>
+      <c r="B29" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="C29" s="21" t="s">
         <v>92</v>
       </c>
@@ -8009,7 +8066,7 @@
       <c r="A30" s="30">
         <v>75967</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="39" t="s">
         <v>125</v>
       </c>
       <c r="C30" s="31" t="s">
@@ -8058,7 +8115,7 @@
     </row>
     <row r="31" spans="1:15" s="24" customFormat="1">
       <c r="A31" s="33"/>
-      <c r="B31" s="46"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="34" t="s">
         <v>96</v>
       </c>
@@ -8227,24 +8284,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
-      <c r="D37" s="25"/>
-      <c r="E37" s="4" t="s">
+    <row r="35" spans="1:15" s="23" customFormat="1">
+      <c r="A35" s="53">
+        <v>76373</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="23">
+        <v>0</v>
+      </c>
+      <c r="E35" s="23">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="24" customFormat="1">
+      <c r="A36" s="54"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="24">
+        <v>512</v>
+      </c>
+      <c r="E36" s="24">
+        <v>188</v>
+      </c>
+      <c r="F36" s="24">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="D38" s="25"/>
+      <c r="E38" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
-      <c r="D38" s="26"/>
-      <c r="E38" s="4" t="s">
+    <row r="39" spans="1:15">
+      <c r="D39" s="26"/>
+      <c r="E39" s="4" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="259" orientation="portrait" r:id="rId1"/>

</xml_diff>